<commit_message>
Deployed to deta spaces
</commit_message>
<xml_diff>
--- a/api/hoja_de_vida/hdv_temp.xlsx
+++ b/api/hoja_de_vida/hdv_temp.xlsx
@@ -1307,7 +1307,7 @@
       <c r="B6" s="114" t="n"/>
       <c r="C6" s="90" t="inlineStr">
         <is>
-          <t>sddsdfs</t>
+          <t>ewrsdfserh</t>
         </is>
       </c>
       <c r="D6" s="111" t="n"/>
@@ -1326,7 +1326,7 @@
       <c r="B7" s="114" t="n"/>
       <c r="C7" s="90" t="inlineStr">
         <is>
-          <t>sddsfsdf</t>
+          <t>vgjbjkb</t>
         </is>
       </c>
       <c r="D7" s="111" t="n"/>
@@ -1345,7 +1345,7 @@
       <c r="B8" s="114" t="n"/>
       <c r="C8" s="90" t="inlineStr">
         <is>
-          <t>qasafs</t>
+          <t>jkjbkjkb</t>
         </is>
       </c>
       <c r="D8" s="111" t="n"/>
@@ -1364,7 +1364,7 @@
       <c r="B9" s="114" t="n"/>
       <c r="C9" s="92" t="inlineStr">
         <is>
-          <t>asasd</t>
+          <t>lkklh</t>
         </is>
       </c>
       <c r="D9" s="111" t="n"/>
@@ -1383,7 +1383,7 @@
       <c r="B10" s="114" t="n"/>
       <c r="C10" s="93" t="inlineStr">
         <is>
-          <t>sdsdfsd</t>
+          <t>klj</t>
         </is>
       </c>
       <c r="D10" s="111" t="n"/>
@@ -1402,7 +1402,7 @@
       <c r="B11" s="114" t="n"/>
       <c r="C11" s="96" t="inlineStr">
         <is>
-          <t>assdf</t>
+          <t>kjljkl</t>
         </is>
       </c>
       <c r="D11" s="111" t="n"/>
@@ -1442,7 +1442,7 @@
       <c r="B13" s="114" t="n"/>
       <c r="C13" s="47" t="inlineStr">
         <is>
-          <t>sdfsdf</t>
+          <t>ñljjñllj</t>
         </is>
       </c>
       <c r="D13" s="111" t="n"/>
@@ -1471,7 +1471,7 @@
       <c r="B14" s="114" t="n"/>
       <c r="C14" s="62" t="inlineStr">
         <is>
-          <t>asas</t>
+          <t>ÑLJÑJLLÑJ</t>
         </is>
       </c>
       <c r="D14" s="114" t="n"/>
@@ -1499,7 +1499,7 @@
       <c r="B15" s="114" t="n"/>
       <c r="C15" s="62" t="inlineStr">
         <is>
-          <t>dddsf</t>
+          <t>JLÑJLÑ</t>
         </is>
       </c>
       <c r="D15" s="114" t="n"/>
@@ -1535,7 +1535,7 @@
       <c r="B16" s="114" t="n"/>
       <c r="C16" s="62" t="inlineStr">
         <is>
-          <t>asasd</t>
+          <t>JLÑLJÑ</t>
         </is>
       </c>
       <c r="D16" s="114" t="n"/>
@@ -1547,7 +1547,7 @@
       <c r="F16" s="114" t="n"/>
       <c r="G16" s="83" t="n"/>
       <c r="H16" s="90" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I16" s="90" t="n">
         <v>8</v>
@@ -1565,7 +1565,7 @@
       <c r="B17" s="114" t="n"/>
       <c r="C17" s="62" t="inlineStr">
         <is>
-          <t>asasf</t>
+          <t>JLÑLJÑ</t>
         </is>
       </c>
       <c r="D17" s="114" t="n"/>
@@ -1577,7 +1577,7 @@
       <c r="F17" s="111" t="n"/>
       <c r="G17" s="114" t="n"/>
       <c r="H17" s="90" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I17" s="90" t="n">
         <v>8</v>
@@ -1595,7 +1595,7 @@
       <c r="B18" s="114" t="n"/>
       <c r="C18" s="62" t="inlineStr">
         <is>
-          <t>asasf</t>
+          <t>JLÑLJ</t>
         </is>
       </c>
       <c r="D18" s="114" t="n"/>
@@ -1607,7 +1607,7 @@
       <c r="F18" s="26" t="n"/>
       <c r="G18" s="26" t="n"/>
       <c r="H18" s="90" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I18" s="90" t="n">
         <v>8</v>
@@ -1625,7 +1625,7 @@
       <c r="B19" s="114" t="n"/>
       <c r="C19" s="121" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>ÑJLÑ</t>
         </is>
       </c>
       <c r="D19" s="114" t="n"/>
@@ -1637,7 +1637,7 @@
       <c r="F19" s="111" t="n"/>
       <c r="G19" s="114" t="n"/>
       <c r="H19" s="90" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I19" s="90" t="n">
         <v>8</v>
@@ -1655,7 +1655,7 @@
       <c r="B20" s="22" t="n"/>
       <c r="C20" s="62" t="inlineStr">
         <is>
-          <t>asas</t>
+          <t>LJÑLJÑ</t>
         </is>
       </c>
       <c r="D20" s="114" t="n"/>
@@ -1715,7 +1715,7 @@
       <c r="B23" s="114" t="n"/>
       <c r="C23" s="75" t="inlineStr">
         <is>
-          <t>sdsdf</t>
+          <t>LJLÑJLJÑ</t>
         </is>
       </c>
       <c r="D23" s="114" t="n"/>
@@ -1727,7 +1727,7 @@
       <c r="F23" s="114" t="n"/>
       <c r="G23" s="18" t="inlineStr">
         <is>
-          <t>asasf</t>
+          <t>JLLJÑÑLJ</t>
         </is>
       </c>
       <c r="H23" s="96" t="inlineStr">
@@ -1738,7 +1738,7 @@
       <c r="I23" s="114" t="n"/>
       <c r="J23" s="17" t="inlineStr">
         <is>
-          <t>dfsdf</t>
+          <t>JLÑJLÑ</t>
         </is>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       <c r="B24" s="114" t="n"/>
       <c r="C24" s="75" t="inlineStr">
         <is>
-          <t>sdsf</t>
+          <t>JLJLÑ</t>
         </is>
       </c>
       <c r="D24" s="114" t="n"/>
@@ -1763,7 +1763,7 @@
       <c r="F24" s="114" t="n"/>
       <c r="G24" s="18" t="inlineStr">
         <is>
-          <t>assdf</t>
+          <t>LJÑ</t>
         </is>
       </c>
       <c r="H24" s="96" t="inlineStr">
@@ -1774,7 +1774,7 @@
       <c r="I24" s="114" t="n"/>
       <c r="J24" s="17" t="inlineStr">
         <is>
-          <t>sddsf</t>
+          <t>LJÑ</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       <c r="B25" s="114" t="n"/>
       <c r="C25" s="75" t="inlineStr">
         <is>
-          <t>dsf</t>
+          <t>JLÑLÑJ</t>
         </is>
       </c>
       <c r="D25" s="114" t="n"/>
@@ -1799,7 +1799,7 @@
       <c r="F25" s="114" t="n"/>
       <c r="G25" s="16" t="inlineStr">
         <is>
-          <t>sdfds</t>
+          <t>KJ</t>
         </is>
       </c>
       <c r="H25" s="124" t="inlineStr">
@@ -1810,7 +1810,7 @@
       <c r="I25" s="114" t="n"/>
       <c r="J25" s="15" t="inlineStr">
         <is>
-          <t>sfd</t>
+          <t>LJÑ</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       <c r="G27" s="114" t="n"/>
       <c r="H27" s="64" t="inlineStr">
         <is>
-          <t>sdfdsf</t>
+          <t>ÑLJJK</t>
         </is>
       </c>
       <c r="I27" s="111" t="n"/>
@@ -1884,7 +1884,7 @@
       <c r="G28" s="114" t="n"/>
       <c r="H28" s="64" t="inlineStr">
         <is>
-          <t>sdsfd</t>
+          <t>IHIH</t>
         </is>
       </c>
       <c r="I28" s="111" t="n"/>
@@ -1912,7 +1912,7 @@
       <c r="G29" s="114" t="n"/>
       <c r="H29" s="64" t="inlineStr">
         <is>
-          <t>sdsdf</t>
+          <t>LKHLKHKL</t>
         </is>
       </c>
       <c r="I29" s="111" t="n"/>
@@ -1927,7 +1927,7 @@
       <c r="B30" s="114" t="n"/>
       <c r="C30" s="64" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>12</t>
         </is>
       </c>
       <c r="D30" s="114" t="n"/>
@@ -1940,7 +1940,7 @@
       <c r="G30" s="114" t="n"/>
       <c r="H30" s="64" t="inlineStr">
         <is>
-          <t>sdsdf</t>
+          <t>KHLHKHKL</t>
         </is>
       </c>
       <c r="I30" s="111" t="n"/>
@@ -1968,7 +1968,7 @@
       <c r="G31" s="114" t="n"/>
       <c r="H31" s="64" t="inlineStr">
         <is>
-          <t>sfsdsd</t>
+          <t>KHLKHL</t>
         </is>
       </c>
       <c r="I31" s="111" t="n"/>
@@ -2021,14 +2021,14 @@
       <c r="D34" s="114" t="n"/>
       <c r="E34" s="63" t="inlineStr">
         <is>
-          <t>CUATRIMESTRAL</t>
+          <t>TRIMESTRAL</t>
         </is>
       </c>
       <c r="F34" s="111" t="n"/>
       <c r="G34" s="114" t="n"/>
       <c r="H34" s="63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I34" s="111" t="n"/>
@@ -2053,7 +2053,7 @@
     <row r="36" ht="20.25" customHeight="1">
       <c r="A36" s="62" t="inlineStr">
         <is>
-          <t>sdfdsfdsf</t>
+          <t>KÑJHLK</t>
         </is>
       </c>
       <c r="B36" s="111" t="n"/>
@@ -2061,7 +2061,7 @@
       <c r="D36" s="114" t="n"/>
       <c r="E36" s="62" t="inlineStr">
         <is>
-          <t>oihio</t>
+          <t xml:space="preserve">4. </t>
         </is>
       </c>
       <c r="F36" s="111" t="n"/>
@@ -2073,7 +2073,7 @@
     <row r="37" ht="18.75" customHeight="1">
       <c r="A37" s="62" t="inlineStr">
         <is>
-          <t>sddfdso</t>
+          <t>ÑLKÑJLÑJ</t>
         </is>
       </c>
       <c r="B37" s="111" t="n"/>
@@ -2081,7 +2081,7 @@
       <c r="D37" s="114" t="n"/>
       <c r="E37" s="62" t="inlineStr">
         <is>
-          <t>hiohoi</t>
+          <t xml:space="preserve">5. </t>
         </is>
       </c>
       <c r="F37" s="111" t="n"/>
@@ -2093,7 +2093,7 @@
     <row r="38" ht="17.25" customHeight="1">
       <c r="A38" s="62" t="inlineStr">
         <is>
-          <t>iohoh</t>
+          <t>LJKLÑJLÑÑJL</t>
         </is>
       </c>
       <c r="B38" s="111" t="n"/>
@@ -2101,7 +2101,7 @@
       <c r="D38" s="114" t="n"/>
       <c r="E38" s="62" t="inlineStr">
         <is>
-          <t>hiohi</t>
+          <t>6.</t>
         </is>
       </c>
       <c r="F38" s="111" t="n"/>

</xml_diff>